<commit_message>
Cleanup. Added supplementary data.
</commit_message>
<xml_diff>
--- a/etc/sbml/Chlamydomonas reinhardtii/kegg_ids.xlsx
+++ b/etc/sbml/Chlamydomonas reinhardtii/kegg_ids.xlsx
@@ -8144,8 +8144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1707"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1689" workbookViewId="0">
-      <selection activeCell="H1696" sqref="H1696:H1707"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H1707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44136,6 +44136,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>